<commit_message>
Update Chiro ODK form
</commit_message>
<xml_diff>
--- a/chiro/odk_form/form_odk_chiro.xlsx
+++ b/chiro/odk_form/form_odk_chiro.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="275">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -262,7 +262,7 @@
     <t xml:space="preserve">begin repeat</t>
   </si>
   <si>
-    <t xml:space="preserve">observer</t>
+    <t xml:space="preserve">observers</t>
   </si>
   <si>
     <t xml:space="preserve">Observat.eur.rice.s</t>
@@ -353,7 +353,7 @@
     <t xml:space="preserve">Boucle pour renseigner l(es) observation(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">observation</t>
+    <t xml:space="preserve">observations</t>
   </si>
   <si>
     <t xml:space="preserve">Espèce(s) observées</t>
@@ -810,6 +810,9 @@
     <t xml:space="preserve">visit.observer</t>
   </si>
   <si>
+    <t xml:space="preserve">observer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nom de la boucle</t>
   </si>
   <si>
@@ -833,6 +836,9 @@
   </si>
   <si>
     <t xml:space="preserve">medias_visit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">observation</t>
   </si>
   <si>
     <t xml:space="preserve">Valeur = taxref.cd_nom</t>
@@ -1400,10 +1406,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
+      <selection pane="bottomLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.55"/>
@@ -2806,7 +2812,7 @@
       <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.78"/>
@@ -3284,7 +3290,7 @@
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.89"/>
@@ -3351,12 +3357,12 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="17.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="44.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="34" width="11.55"/>
@@ -3556,24 +3562,24 @@
         <v>257</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>76</v>
+        <v>258</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
       <c r="E16" s="38"/>
       <c r="F16" s="38" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B17" s="37" t="s">
         <v>80</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D17" s="38" t="s">
         <v>242</v>
@@ -3585,7 +3591,7 @@
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>66</v>
@@ -3596,12 +3602,12 @@
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="38" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B19" s="37" t="s">
         <v>72</v>
@@ -3612,12 +3618,12 @@
       </c>
       <c r="E19" s="38"/>
       <c r="F19" s="38" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B20" s="37" t="s">
         <v>101</v>
@@ -3631,10 +3637,10 @@
     </row>
     <row r="21" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C21" s="38"/>
       <c r="D21" s="38" t="s">
@@ -3644,15 +3650,15 @@
         <v>99999</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B22" s="37" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="38" t="s">
@@ -3663,7 +3669,7 @@
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="36" t="s">
-        <v>106</v>
+        <v>267</v>
       </c>
       <c r="B23" s="37" t="s">
         <v>113</v>
@@ -3674,12 +3680,12 @@
       </c>
       <c r="E23" s="38"/>
       <c r="F23" s="38" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="36" t="s">
-        <v>106</v>
+        <v>267</v>
       </c>
       <c r="B24" s="37" t="s">
         <v>147</v>
@@ -3693,7 +3699,7 @@
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="36" t="s">
-        <v>106</v>
+        <v>267</v>
       </c>
       <c r="B25" s="37" t="s">
         <v>152</v>
@@ -3727,7 +3733,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3766,30 +3772,30 @@
   <sheetData>
     <row r="1" s="41" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="41" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B1" s="41" t="s">
         <v>249</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="40" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B2" s="42" t="n">
         <v>44904</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>